<commit_message>
Updated list of murals in Ursynów
</commit_message>
<xml_diff>
--- a/data/interim/murale_ursynow.xlsx
+++ b/data/interim/murale_ursynow.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Pulpit\Projekty\Unemployment\data\interim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Pulpit\Projekty\murals\data\interim\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
   <si>
     <t>lat</t>
   </si>
@@ -47,9 +47,6 @@
     <t xml:space="preserve"> 21.035278</t>
   </si>
   <si>
-    <t xml:space="preserve"> 21.035803</t>
-  </si>
-  <si>
     <t>52.155711</t>
   </si>
   <si>
@@ -60,13 +57,325 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>001_ludzikowie_ wiolinowa_14</t>
+  </si>
+  <si>
+    <t>002_mis_i_motyl-meander_16</t>
+  </si>
+  <si>
+    <t>003_tygrys-warchalowskiego_4</t>
+  </si>
+  <si>
+    <t>004_calineczka-polinezyjska_6</t>
+  </si>
+  <si>
+    <t>005_ptaki-na_uboczu_4</t>
+  </si>
+  <si>
+    <t>006_gospodarz-kazury_10</t>
+  </si>
+  <si>
+    <t>007_jerzykiada-koński_jar_8</t>
+  </si>
+  <si>
+    <t>008_rezerwat-koński_jar_3</t>
+  </si>
+  <si>
+    <t>009_wiezniarka-hirszfelda_11</t>
+  </si>
+  <si>
+    <t>010_jaskolki-nutki_1</t>
+  </si>
+  <si>
+    <t>011_pilecki-pileckiego_111</t>
+  </si>
+  <si>
+    <t>012_mala_laka-malej_laki_7</t>
+  </si>
+  <si>
+    <t>013_magellan-magellana_2</t>
+  </si>
+  <si>
+    <t>015_ursyn_niemcewicz-metro_imelin</t>
+  </si>
+  <si>
+    <t>016_grzegorzewska-metro_imelin</t>
+  </si>
+  <si>
+    <t>017_spiaca_syrenka-teligi_2</t>
+  </si>
+  <si>
+    <t>019_stryjenska-kazury_8</t>
+  </si>
+  <si>
+    <t>020_ursynow-malej_laki_21</t>
+  </si>
+  <si>
+    <t>021_deyna-kazury_16</t>
+  </si>
+  <si>
+    <t>022_40_latek-metro_ursynów</t>
+  </si>
+  <si>
+    <t>023_plan_zdjeciowy-grzegorzewskiej_3</t>
+  </si>
+  <si>
+    <t>024_klatka-grzegorzewskiej_1</t>
+  </si>
+  <si>
+    <t>025_pachnaca-rosola</t>
+  </si>
+  <si>
+    <t>028_hospicjum-pileckigo_105</t>
+  </si>
+  <si>
+    <t>029_kosmowska-sarabandy_16</t>
+  </si>
+  <si>
+    <t>ludzikowie</t>
+  </si>
+  <si>
+    <t>gospodarz-kazury</t>
+  </si>
+  <si>
+    <t>jerzykiada-koński</t>
+  </si>
+  <si>
+    <t>rezerwat-koński</t>
+  </si>
+  <si>
+    <t>pachnaca</t>
+  </si>
+  <si>
+    <t>mis_i_motyl</t>
+  </si>
+  <si>
+    <t>tygrys</t>
+  </si>
+  <si>
+    <t>calineczka</t>
+  </si>
+  <si>
+    <t>wiezniarka</t>
+  </si>
+  <si>
+    <t>jaskolki</t>
+  </si>
+  <si>
+    <t>magellan</t>
+  </si>
+  <si>
+    <t>spiaca_syrenka</t>
+  </si>
+  <si>
+    <t>stryjenska</t>
+  </si>
+  <si>
+    <t>deyna</t>
+  </si>
+  <si>
+    <t>plan_zdjeciowy</t>
+  </si>
+  <si>
+    <t>klatka</t>
+  </si>
+  <si>
+    <t>hospicjum</t>
+  </si>
+  <si>
+    <t>kosmowska</t>
+  </si>
+  <si>
+    <t>mala_laka</t>
+  </si>
+  <si>
+    <t>ursyn_niemcewicz</t>
+  </si>
+  <si>
+    <t>grzegorzewska</t>
+  </si>
+  <si>
+    <t>ursynow</t>
+  </si>
+  <si>
+    <t>40_latek</t>
+  </si>
+  <si>
+    <t>ptaki-na_uboczu</t>
+  </si>
+  <si>
+    <t>52.1614339</t>
+  </si>
+  <si>
+    <t>21.0267905</t>
+  </si>
+  <si>
+    <t>52.1419292</t>
+  </si>
+  <si>
+    <t>21.0549329</t>
+  </si>
+  <si>
+    <t>21.045374</t>
+  </si>
+  <si>
+    <t>52.145036</t>
+  </si>
+  <si>
+    <t>52.151709</t>
+  </si>
+  <si>
+    <t>21.0456892</t>
+  </si>
+  <si>
+    <t>21.0502505</t>
+  </si>
+  <si>
+    <t>52.1395759</t>
+  </si>
+  <si>
+    <t>52.1407999</t>
+  </si>
+  <si>
+    <t>21.0440443</t>
+  </si>
+  <si>
+    <t>52.164364</t>
+  </si>
+  <si>
+    <t>21.0236323</t>
+  </si>
+  <si>
+    <t>52.1628015</t>
+  </si>
+  <si>
+    <t>21.0231137</t>
+  </si>
+  <si>
+    <t>52.1438551</t>
+  </si>
+  <si>
+    <t>21.0378979</t>
+  </si>
+  <si>
+    <t>52.1621212</t>
+  </si>
+  <si>
+    <t>21.019935</t>
+  </si>
+  <si>
+    <t>52.1416947</t>
+  </si>
+  <si>
+    <t>21.0352853</t>
+  </si>
+  <si>
+    <t>52.1365522</t>
+  </si>
+  <si>
+    <t>21.0513092</t>
+  </si>
+  <si>
+    <t>52.1537027</t>
+  </si>
+  <si>
+    <t>21.0449176</t>
+  </si>
+  <si>
+    <t>21.035803</t>
+  </si>
+  <si>
+    <t>21.047075</t>
+  </si>
+  <si>
+    <t>52.148500</t>
+  </si>
+  <si>
+    <t>52.148693</t>
+  </si>
+  <si>
+    <t>21.047413</t>
+  </si>
+  <si>
+    <t>52.153857</t>
+  </si>
+  <si>
+    <t>21.0462999</t>
+  </si>
+  <si>
+    <t>52.1407547</t>
+  </si>
+  <si>
+    <t>21.0435995</t>
+  </si>
+  <si>
+    <t>52.1370963</t>
+  </si>
+  <si>
+    <t>21.0485083</t>
+  </si>
+  <si>
+    <t>52.1402553</t>
+  </si>
+  <si>
+    <t>21.0398211</t>
+  </si>
+  <si>
+    <t>52.161319</t>
+  </si>
+  <si>
+    <t>21.028184</t>
+  </si>
+  <si>
+    <t>52.1497478</t>
+  </si>
+  <si>
+    <t>21.0540321</t>
+  </si>
+  <si>
+    <t>52.1492373</t>
+  </si>
+  <si>
+    <t>21.0544436</t>
+  </si>
+  <si>
+    <t>21.0617668</t>
+  </si>
+  <si>
+    <t>52.1472054</t>
+  </si>
+  <si>
+    <t>027_takie_panny-szolc_rogozinskiego_10</t>
+  </si>
+  <si>
+    <t>takie_panny</t>
+  </si>
+  <si>
+    <t>21.050853</t>
+  </si>
+  <si>
+    <t>52.1513599</t>
+  </si>
+  <si>
+    <t>52.1435398</t>
+  </si>
+  <si>
+    <t>21.0350314</t>
+  </si>
+  <si>
+    <t>52.1133445</t>
+  </si>
+  <si>
+    <t>21.0120799</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,14 +383,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="7"/>
-      <color rgb="FF4285F4"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,9 +405,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -387,21 +687,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A30" sqref="A30:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
     <col min="4" max="4" width="23.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -415,37 +717,395 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C19" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>